<commit_message>
Actualizacion total de app
</commit_message>
<xml_diff>
--- a/Stock/src/main/resources/layout/LayoutArea.xlsx
+++ b/Stock/src/main/resources/layout/LayoutArea.xlsx
@@ -3,14 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14970" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogo Áreas" sheetId="1" r:id="rId1"/>
+    <sheet name="Almacenes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>SISTEMAS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Contabilidad</t>
   </si>
@@ -35,13 +37,148 @@
   </si>
   <si>
     <t>Administracion</t>
+  </si>
+  <si>
+    <t>Norte</t>
+  </si>
+  <si>
+    <t>Sur</t>
+  </si>
+  <si>
+    <t>Este</t>
+  </si>
+  <si>
+    <t>Oeste</t>
+  </si>
+  <si>
+    <t>Almacen 1</t>
+  </si>
+  <si>
+    <t>Almacen 2</t>
+  </si>
+  <si>
+    <t>Almacen 3</t>
+  </si>
+  <si>
+    <t>Almacen 4</t>
+  </si>
+  <si>
+    <t>Almacen 5</t>
+  </si>
+  <si>
+    <t>Almacen 6</t>
+  </si>
+  <si>
+    <t>Almacen 7</t>
+  </si>
+  <si>
+    <t>Almacen 8</t>
+  </si>
+  <si>
+    <t>Almacen 9</t>
+  </si>
+  <si>
+    <t>Almacen 10</t>
+  </si>
+  <si>
+    <t>Almacen 11</t>
+  </si>
+  <si>
+    <t>Almacen 12</t>
+  </si>
+  <si>
+    <t>Almacen 13</t>
+  </si>
+  <si>
+    <t>Almacen 14</t>
+  </si>
+  <si>
+    <t>Almacen 15</t>
+  </si>
+  <si>
+    <t>Almacen 16</t>
+  </si>
+  <si>
+    <t>Almacen 17</t>
+  </si>
+  <si>
+    <t>Almacen 18</t>
+  </si>
+  <si>
+    <t>Almacen 19</t>
+  </si>
+  <si>
+    <t>Almacen 20</t>
+  </si>
+  <si>
+    <t>Almacen 21</t>
+  </si>
+  <si>
+    <t>Almacen 22</t>
+  </si>
+  <si>
+    <t>Almacen 23</t>
+  </si>
+  <si>
+    <t>Almacen 24</t>
+  </si>
+  <si>
+    <t>Almacen 25</t>
+  </si>
+  <si>
+    <t>Almacen 26</t>
+  </si>
+  <si>
+    <t>Almacen 27</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Westwood</t>
+  </si>
+  <si>
+    <t>Exclusiva</t>
+  </si>
+  <si>
+    <t>Fantastique</t>
+  </si>
+  <si>
+    <t>Magnum</t>
+  </si>
+  <si>
+    <t>Jolie</t>
+  </si>
+  <si>
+    <t>Galeria</t>
+  </si>
+  <si>
+    <t>Glamour</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Casual livin'</t>
+  </si>
+  <si>
+    <t>Sistemas</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +190,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,12 +234,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,30 +541,502 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="6">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>